<commit_message>
fix test problem on importing xlsx
</commit_message>
<xml_diff>
--- a/spp_event_demo/tests/import_data/house_visit.xlsx
+++ b/spp_event_demo/tests/import_data/house_visit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpaul\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpaul\Michael\OpenSPP\openspp-registry\spp_event_demo\tests\import_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B48CBB-7C8E-4FCE-A414-301E78C7A6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5ECE7D-E85A-46EA-871B-DE5441D73127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="3825" windowWidth="21600" windowHeight="11835" xr2:uid="{54ACA00C-4226-4E2E-A7EA-9EC9AA5C0E19}"/>
+    <workbookView xWindow="3240" yWindow="3645" windowWidth="21600" windowHeight="11835" xr2:uid="{54ACA00C-4226-4E2E-A7EA-9EC9AA5C0E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,10 +473,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>

</xml_diff>